<commit_message>
add oto360, improve hohh script
</commit_message>
<xml_diff>
--- a/Object Repository.xlsx
+++ b/Object Repository.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15530" windowHeight="6930"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="15530" windowHeight="6930" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamic" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="316">
   <si>
     <t>Product</t>
   </si>
@@ -897,6 +897,84 @@
   </si>
   <si>
     <t>NRIC no.</t>
+  </si>
+  <si>
+    <t>Please enter your Vehicle Number</t>
+  </si>
+  <si>
+    <t>wrnmsg.vehicleNumber</t>
+  </si>
+  <si>
+    <t>detail.quotationVehicleNumber</t>
+  </si>
+  <si>
+    <t>detail.quotationPassport</t>
+  </si>
+  <si>
+    <t>Passport no.</t>
+  </si>
+  <si>
+    <t>Date of Birth (DD/MM/YYYY)</t>
+  </si>
+  <si>
+    <t>detail.quotationDateOfBirth</t>
+  </si>
+  <si>
+    <t>ID No.</t>
+  </si>
+  <si>
+    <t>detail.quotationID</t>
+  </si>
+  <si>
+    <t>detail.quotationEmail</t>
+  </si>
+  <si>
+    <t>detail.name</t>
+  </si>
+  <si>
+    <t>Name (as per NRIC)</t>
+  </si>
+  <si>
+    <t>detail.dateOfBirth</t>
+  </si>
+  <si>
+    <t>detail.mobileNumber</t>
+  </si>
+  <si>
+    <t>Address 1</t>
+  </si>
+  <si>
+    <t>detail.address1</t>
+  </si>
+  <si>
+    <t>detail.address2</t>
+  </si>
+  <si>
+    <t>Address 2</t>
+  </si>
+  <si>
+    <t>City (Optional)</t>
+  </si>
+  <si>
+    <t>detail.city</t>
+  </si>
+  <si>
+    <t>detail.postcode</t>
+  </si>
+  <si>
+    <t>detail.state</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Current / Saving Account no.</t>
+  </si>
+  <si>
+    <t>detail.savingAccount</t>
+  </si>
+  <si>
+    <t>detail.country</t>
   </si>
 </sst>
 </file>
@@ -1226,10 +1304,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D119"/>
+  <dimension ref="A1:D135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E109" sqref="E109"/>
+    <sheetView topLeftCell="A76" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2550,6 +2628,182 @@
         <v>289</v>
       </c>
     </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
+        <v>196</v>
+      </c>
+      <c r="B120" t="s">
+        <v>291</v>
+      </c>
+      <c r="C120" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
+        <v>196</v>
+      </c>
+      <c r="B121" t="s">
+        <v>292</v>
+      </c>
+      <c r="C121" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
+        <v>196</v>
+      </c>
+      <c r="B122" t="s">
+        <v>293</v>
+      </c>
+      <c r="C122" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
+        <v>196</v>
+      </c>
+      <c r="B123" t="s">
+        <v>296</v>
+      </c>
+      <c r="C123" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>196</v>
+      </c>
+      <c r="B124" t="s">
+        <v>298</v>
+      </c>
+      <c r="C124" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
+        <v>196</v>
+      </c>
+      <c r="B125" t="s">
+        <v>299</v>
+      </c>
+      <c r="C125" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
+        <v>196</v>
+      </c>
+      <c r="B126" t="s">
+        <v>300</v>
+      </c>
+      <c r="C126" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
+        <v>196</v>
+      </c>
+      <c r="B127" t="s">
+        <v>302</v>
+      </c>
+      <c r="C127" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
+        <v>196</v>
+      </c>
+      <c r="B128" t="s">
+        <v>303</v>
+      </c>
+      <c r="C128" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
+        <v>196</v>
+      </c>
+      <c r="B129" t="s">
+        <v>305</v>
+      </c>
+      <c r="C129" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
+        <v>196</v>
+      </c>
+      <c r="B130" t="s">
+        <v>306</v>
+      </c>
+      <c r="C130" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
+        <v>196</v>
+      </c>
+      <c r="B131" t="s">
+        <v>309</v>
+      </c>
+      <c r="C131" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
+        <v>196</v>
+      </c>
+      <c r="B132" t="s">
+        <v>310</v>
+      </c>
+      <c r="C132" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
+        <v>196</v>
+      </c>
+      <c r="B133" t="s">
+        <v>311</v>
+      </c>
+      <c r="C133" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
+        <v>196</v>
+      </c>
+      <c r="B134" t="s">
+        <v>315</v>
+      </c>
+      <c r="C134" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
+        <v>196</v>
+      </c>
+      <c r="B135" t="s">
+        <v>314</v>
+      </c>
+      <c r="C135" t="s">
+        <v>313</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2561,7 +2815,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2765,8 +3019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
change test case name
</commit_message>
<xml_diff>
--- a/Object Repository.xlsx
+++ b/Object Repository.xlsx
@@ -15,7 +15,8 @@
     <sheet name="Dynamic" sheetId="1" r:id="rId1"/>
     <sheet name="TravellerInfo" sheetId="2" r:id="rId2"/>
     <sheet name="OTO360" sheetId="3" r:id="rId3"/>
-    <sheet name="BankInfo" sheetId="4" r:id="rId4"/>
+    <sheet name="MyRumah" sheetId="5" r:id="rId4"/>
+    <sheet name="BankInfo" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="336">
   <si>
     <t>Product</t>
   </si>
@@ -761,63 +762,264 @@
     <t>Set1</t>
   </si>
   <si>
+    <t>passportNo</t>
+  </si>
+  <si>
+    <t>dateOfBirth</t>
+  </si>
+  <si>
+    <t>emailForRenewal</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>race</t>
+  </si>
+  <si>
+    <t>mobileNumber</t>
+  </si>
+  <si>
+    <t>address1</t>
+  </si>
+  <si>
+    <t>address2</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>bankName</t>
+  </si>
+  <si>
+    <t>savingAccount</t>
+  </si>
+  <si>
+    <t>userId</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Lee Ong Lim</t>
+  </si>
+  <si>
+    <t>A12345678</t>
+  </si>
+  <si>
+    <t>text.quotationForm</t>
+  </si>
+  <si>
+    <t>Enhance Your Motor Coverage Now</t>
+  </si>
+  <si>
+    <t>submit.quotationCheck</t>
+  </si>
+  <si>
+    <t>Apply Now</t>
+  </si>
+  <si>
+    <t>quotation.nationality</t>
+  </si>
+  <si>
+    <t>Your current coverage is still active</t>
+  </si>
+  <si>
+    <t>Please fill in your vehicle details</t>
+  </si>
+  <si>
+    <t>text.vehicleNotEligible</t>
+  </si>
+  <si>
+    <t>text.vehicleEligible</t>
+  </si>
+  <si>
+    <t>submit.sendEmailRenewal</t>
+  </si>
+  <si>
+    <t>Remind me</t>
+  </si>
+  <si>
+    <t>Thank you, we have received your request!</t>
+  </si>
+  <si>
+    <t>text.receivedRequest</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>currentSite.review</t>
+  </si>
+  <si>
+    <t>Fill Up Details</t>
+  </si>
+  <si>
+    <t>Summary &amp; Payment</t>
+  </si>
+  <si>
+    <t>Please choose the payment option below</t>
+  </si>
+  <si>
+    <t>Please enter your 12-digit NRIC number, e.g., 771111101233</t>
+  </si>
+  <si>
+    <t>wrnmsg.ic</t>
+  </si>
+  <si>
+    <t>detail.ic</t>
+  </si>
+  <si>
+    <t>NRIC no.</t>
+  </si>
+  <si>
+    <t>Please enter your Vehicle Number</t>
+  </si>
+  <si>
+    <t>wrnmsg.vehicleNumber</t>
+  </si>
+  <si>
+    <t>detail.quotationVehicleNumber</t>
+  </si>
+  <si>
+    <t>detail.quotationPassport</t>
+  </si>
+  <si>
+    <t>Passport no.</t>
+  </si>
+  <si>
+    <t>Date of Birth (DD/MM/YYYY)</t>
+  </si>
+  <si>
+    <t>detail.quotationDateOfBirth</t>
+  </si>
+  <si>
+    <t>ID No.</t>
+  </si>
+  <si>
+    <t>detail.quotationID</t>
+  </si>
+  <si>
+    <t>detail.quotationEmail</t>
+  </si>
+  <si>
+    <t>detail.name</t>
+  </si>
+  <si>
+    <t>Name (as per NRIC)</t>
+  </si>
+  <si>
+    <t>detail.dateOfBirth</t>
+  </si>
+  <si>
+    <t>detail.mobileNumber</t>
+  </si>
+  <si>
+    <t>Address 1</t>
+  </si>
+  <si>
+    <t>detail.address1</t>
+  </si>
+  <si>
+    <t>detail.address2</t>
+  </si>
+  <si>
+    <t>Address 2</t>
+  </si>
+  <si>
+    <t>City (Optional)</t>
+  </si>
+  <si>
+    <t>detail.city</t>
+  </si>
+  <si>
+    <t>detail.postcode</t>
+  </si>
+  <si>
+    <t>detail.state</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Current / Saving Account no.</t>
+  </si>
+  <si>
+    <t>detail.savingAccount</t>
+  </si>
+  <si>
+    <t>detail.country</t>
+  </si>
+  <si>
+    <t>Mobile number</t>
+  </si>
+  <si>
+    <t>MyRumah</t>
+  </si>
+  <si>
+    <t>submit.checkFlood</t>
+  </si>
+  <si>
+    <t>Check now</t>
+  </si>
+  <si>
+    <t>submit.viewProduct</t>
+  </si>
+  <si>
+    <t>View full product details</t>
+  </si>
+  <si>
+    <t>text.isFlooding</t>
+  </si>
+  <si>
+    <t>text.isUnoccupied</t>
+  </si>
+  <si>
+    <t>text.isSuffered</t>
+  </si>
+  <si>
+    <t>text.isRegistered</t>
+  </si>
+  <si>
+    <t>Is your property currently experiencing flooding?</t>
+  </si>
+  <si>
+    <t>Will this property be unoccupied for 90 days or more?</t>
+  </si>
+  <si>
+    <t>Have you suffered any loss or damage on this property in the past two years?</t>
+  </si>
+  <si>
+    <t>Is the property registered under your name as the house owner?</t>
+  </si>
+  <si>
+    <t>quotation.yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>quotation.no</t>
+  </si>
+  <si>
+    <t>51200</t>
+  </si>
+  <si>
+    <t>Key in your postcode to check for flood risk.</t>
+  </si>
+  <si>
+    <t>text.postcode</t>
+  </si>
+  <si>
     <t>vehicleNumber</t>
   </si>
   <si>
-    <t>passportNo</t>
-  </si>
-  <si>
-    <t>dateOfBirth</t>
-  </si>
-  <si>
-    <t>emailForRenewal</t>
-  </si>
-  <si>
     <t>promotionSelection</t>
   </si>
   <si>
     <t>planClass</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>race</t>
-  </si>
-  <si>
-    <t>mobileNumber</t>
-  </si>
-  <si>
-    <t>address1</t>
-  </si>
-  <si>
-    <t>address2</t>
-  </si>
-  <si>
-    <t>city</t>
-  </si>
-  <si>
-    <t>bankName</t>
-  </si>
-  <si>
-    <t>savingAccount</t>
-  </si>
-  <si>
-    <t>userId</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>Lee Ong Lim</t>
-  </si>
-  <si>
-    <t>VOA0005</t>
-  </si>
-  <si>
-    <t>A12345678</t>
-  </si>
-  <si>
     <t>RF/123456</t>
   </si>
   <si>
@@ -833,151 +1035,7 @@
     <t>idType</t>
   </si>
   <si>
-    <t>text.quotationForm</t>
-  </si>
-  <si>
-    <t>Enhance Your Motor Coverage Now</t>
-  </si>
-  <si>
-    <t>submit.quotationCheck</t>
-  </si>
-  <si>
-    <t>Apply Now</t>
-  </si>
-  <si>
-    <t>quotation.nationality</t>
-  </si>
-  <si>
-    <t>Your current coverage is still active</t>
-  </si>
-  <si>
-    <t>Please fill in your vehicle details</t>
-  </si>
-  <si>
-    <t>text.vehicleNotEligible</t>
-  </si>
-  <si>
-    <t>text.vehicleEligible</t>
-  </si>
-  <si>
-    <t>submit.sendEmailRenewal</t>
-  </si>
-  <si>
-    <t>Remind me</t>
-  </si>
-  <si>
-    <t>Thank you, we have received your request!</t>
-  </si>
-  <si>
-    <t>text.receivedRequest</t>
-  </si>
-  <si>
-    <t>gender</t>
-  </si>
-  <si>
-    <t>currentSite.review</t>
-  </si>
-  <si>
-    <t>Fill Up Details</t>
-  </si>
-  <si>
-    <t>Summary &amp; Payment</t>
-  </si>
-  <si>
-    <t>Please choose the payment option below</t>
-  </si>
-  <si>
-    <t>Please enter your 12-digit NRIC number, e.g., 771111101233</t>
-  </si>
-  <si>
-    <t>wrnmsg.ic</t>
-  </si>
-  <si>
-    <t>detail.ic</t>
-  </si>
-  <si>
-    <t>NRIC no.</t>
-  </si>
-  <si>
-    <t>Please enter your Vehicle Number</t>
-  </si>
-  <si>
-    <t>wrnmsg.vehicleNumber</t>
-  </si>
-  <si>
-    <t>detail.quotationVehicleNumber</t>
-  </si>
-  <si>
-    <t>detail.quotationPassport</t>
-  </si>
-  <si>
-    <t>Passport no.</t>
-  </si>
-  <si>
-    <t>Date of Birth (DD/MM/YYYY)</t>
-  </si>
-  <si>
-    <t>detail.quotationDateOfBirth</t>
-  </si>
-  <si>
-    <t>ID No.</t>
-  </si>
-  <si>
-    <t>detail.quotationID</t>
-  </si>
-  <si>
-    <t>detail.quotationEmail</t>
-  </si>
-  <si>
-    <t>detail.name</t>
-  </si>
-  <si>
-    <t>Name (as per NRIC)</t>
-  </si>
-  <si>
-    <t>detail.dateOfBirth</t>
-  </si>
-  <si>
-    <t>detail.mobileNumber</t>
-  </si>
-  <si>
-    <t>Address 1</t>
-  </si>
-  <si>
-    <t>detail.address1</t>
-  </si>
-  <si>
-    <t>detail.address2</t>
-  </si>
-  <si>
-    <t>Address 2</t>
-  </si>
-  <si>
-    <t>City (Optional)</t>
-  </si>
-  <si>
-    <t>detail.city</t>
-  </si>
-  <si>
-    <t>detail.postcode</t>
-  </si>
-  <si>
-    <t>detail.state</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>Current / Saving Account no.</t>
-  </si>
-  <si>
-    <t>detail.savingAccount</t>
-  </si>
-  <si>
-    <t>detail.country</t>
-  </si>
-  <si>
-    <t>Mobile number</t>
+    <t>VOA0015</t>
   </si>
 </sst>
 </file>
@@ -1307,14 +1365,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D135"/>
+  <dimension ref="A1:D146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G114" sqref="G114"/>
+    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C153" sqref="C153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="9.7265625" customWidth="1"/>
     <col min="2" max="2" width="30.6328125" customWidth="1"/>
     <col min="3" max="3" width="104.81640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -2251,7 +2310,7 @@
         <v>196</v>
       </c>
       <c r="B85" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="C85" t="s">
         <v>47</v>
@@ -2493,10 +2552,10 @@
         <v>196</v>
       </c>
       <c r="B107" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="C107" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
@@ -2504,10 +2563,10 @@
         <v>196</v>
       </c>
       <c r="B108" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="C108" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
@@ -2515,10 +2574,10 @@
         <v>196</v>
       </c>
       <c r="B109" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="C109" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
@@ -2526,10 +2585,10 @@
         <v>196</v>
       </c>
       <c r="B110" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="C110" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
@@ -2537,10 +2596,10 @@
         <v>196</v>
       </c>
       <c r="B111" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="C111" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
@@ -2548,10 +2607,10 @@
         <v>196</v>
       </c>
       <c r="B112" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="C112" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
@@ -2573,7 +2632,7 @@
         <v>67</v>
       </c>
       <c r="C114" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
@@ -2581,10 +2640,10 @@
         <v>196</v>
       </c>
       <c r="B115" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="C115" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
@@ -2606,7 +2665,7 @@
         <v>142</v>
       </c>
       <c r="C117" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.35">
@@ -2614,10 +2673,10 @@
         <v>196</v>
       </c>
       <c r="B118" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="C118" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.35">
@@ -2625,10 +2684,10 @@
         <v>196</v>
       </c>
       <c r="B119" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="C119" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.35">
@@ -2636,10 +2695,10 @@
         <v>196</v>
       </c>
       <c r="B120" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="C120" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.35">
@@ -2647,7 +2706,7 @@
         <v>196</v>
       </c>
       <c r="B121" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="C121" t="s">
         <v>213</v>
@@ -2658,10 +2717,10 @@
         <v>196</v>
       </c>
       <c r="B122" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="C122" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.35">
@@ -2669,10 +2728,10 @@
         <v>196</v>
       </c>
       <c r="B123" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="C123" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
@@ -2680,10 +2739,10 @@
         <v>196</v>
       </c>
       <c r="B124" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="C124" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.35">
@@ -2691,7 +2750,7 @@
         <v>196</v>
       </c>
       <c r="B125" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="C125" t="s">
         <v>53</v>
@@ -2702,10 +2761,10 @@
         <v>196</v>
       </c>
       <c r="B126" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="C126" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.35">
@@ -2713,10 +2772,10 @@
         <v>196</v>
       </c>
       <c r="B127" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="C127" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.35">
@@ -2724,10 +2783,10 @@
         <v>196</v>
       </c>
       <c r="B128" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="C128" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.35">
@@ -2735,10 +2794,10 @@
         <v>196</v>
       </c>
       <c r="B129" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="C129" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.35">
@@ -2746,10 +2805,10 @@
         <v>196</v>
       </c>
       <c r="B130" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="C130" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.35">
@@ -2757,10 +2816,10 @@
         <v>196</v>
       </c>
       <c r="B131" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="C131" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.35">
@@ -2768,7 +2827,7 @@
         <v>196</v>
       </c>
       <c r="B132" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="C132" t="s">
         <v>58</v>
@@ -2779,7 +2838,7 @@
         <v>196</v>
       </c>
       <c r="B133" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="C133" t="s">
         <v>59</v>
@@ -2790,10 +2849,10 @@
         <v>196</v>
       </c>
       <c r="B134" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="C134" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.35">
@@ -2801,10 +2860,131 @@
         <v>196</v>
       </c>
       <c r="B135" t="s">
+        <v>305</v>
+      </c>
+      <c r="C135" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
+        <v>308</v>
+      </c>
+      <c r="B136" t="s">
+        <v>309</v>
+      </c>
+      <c r="C136" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
+        <v>308</v>
+      </c>
+      <c r="B137" t="s">
+        <v>239</v>
+      </c>
+      <c r="C137" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
+        <v>308</v>
+      </c>
+      <c r="B138" t="s">
+        <v>311</v>
+      </c>
+      <c r="C138" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
+        <v>308</v>
+      </c>
+      <c r="B139" t="s">
+        <v>313</v>
+      </c>
+      <c r="C139" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>308</v>
+      </c>
+      <c r="B140" t="s">
         <v>314</v>
       </c>
-      <c r="C135" t="s">
-        <v>313</v>
+      <c r="C140" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
+        <v>308</v>
+      </c>
+      <c r="B141" t="s">
+        <v>315</v>
+      </c>
+      <c r="C141" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
+        <v>308</v>
+      </c>
+      <c r="B142" t="s">
+        <v>316</v>
+      </c>
+      <c r="C142" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
+        <v>308</v>
+      </c>
+      <c r="B143" t="s">
+        <v>263</v>
+      </c>
+      <c r="C143" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
+        <v>308</v>
+      </c>
+      <c r="B144" t="s">
+        <v>321</v>
+      </c>
+      <c r="C144" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
+        <v>308</v>
+      </c>
+      <c r="B145" t="s">
+        <v>323</v>
+      </c>
+      <c r="C145" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
+        <v>308</v>
+      </c>
+      <c r="B146" t="s">
+        <v>326</v>
+      </c>
+      <c r="C146" t="s">
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -3023,7 +3203,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="E14" sqref="E14:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3042,7 +3222,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>267</v>
+        <v>334</v>
       </c>
       <c r="B2" t="s">
         <v>199</v>
@@ -3058,23 +3238,23 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>244</v>
+        <v>327</v>
       </c>
       <c r="B4" t="s">
-        <v>261</v>
+        <v>335</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B5" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B6">
         <v>28092000</v>
@@ -3090,23 +3270,23 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>265</v>
+        <v>332</v>
       </c>
       <c r="B8" t="s">
-        <v>263</v>
+        <v>330</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>266</v>
+        <v>333</v>
       </c>
       <c r="B9" t="s">
-        <v>264</v>
+        <v>331</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>166</v>
@@ -3114,12 +3294,12 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>248</v>
+        <v>328</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>249</v>
+        <v>329</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -3127,15 +3307,15 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B13" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B14" t="s">
         <v>229</v>
@@ -3143,7 +3323,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="B15" t="s">
         <v>227</v>
@@ -3151,7 +3331,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B16">
         <v>1139519168</v>
@@ -3167,7 +3347,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B18" t="s">
         <v>168</v>
@@ -3175,7 +3355,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B19" t="s">
         <v>169</v>
@@ -3183,7 +3363,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
@@ -3196,7 +3376,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B22" t="s">
         <v>173</v>
@@ -3204,7 +3384,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>175</v>
@@ -3222,6 +3402,162 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>244</v>
+      </c>
+      <c r="B3" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>245</v>
+      </c>
+      <c r="B4">
+        <v>28092000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>246</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>247</v>
+      </c>
+      <c r="B7" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>248</v>
+      </c>
+      <c r="B8" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>272</v>
+      </c>
+      <c r="B9" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>249</v>
+      </c>
+      <c r="B10">
+        <v>1139519168</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>157</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>250</v>
+      </c>
+      <c r="B12" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>251</v>
+      </c>
+      <c r="B13" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>161</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>253</v>
+      </c>
+      <c r="B16" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>254</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B11" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3240,7 +3576,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B2">
         <v>1111</v>
@@ -3248,7 +3584,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B3">
         <v>1111</v>

</xml_diff>